<commit_message>
desafio 36, testeado router carrito excepto endpoint con req.user
</commit_message>
<xml_diff>
--- a/desafio.clase.36.tercera.preentrega/postman-tercera-entrega.xlsx
+++ b/desafio.clase.36.tercera.preentrega/postman-tercera-entrega.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\desafio.clase.36.tercer.preentrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1005689D-573F-4DF4-9644-D68C0B52FC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C7B8C-3269-40D5-8EC3-1D6C8D5B00E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9C3F8A7-1291-4D19-868D-FE5390AAF598}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E9C3F8A7-1291-4D19-868D-FE5390AAF598}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
+    <sheet name="Carrito" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>Metodo</t>
   </si>
@@ -86,6 +87,60 @@
   </si>
   <si>
     <t>Actualiza propiedades de un producto. Si se ingresa un parametro incorrecto, debe dar mensaje de error (probar con numero y letra). Si se ingresa una propiedad que no existe, debe dar un mensaje de error. Si se ingresa un tipo de dato no admitido, tambien debe dar error.</t>
+  </si>
+  <si>
+    <t>Devuelve todos los carritos. Una vez finalizado el proyecto, este endpoint DEBE ELIMINARSE</t>
+  </si>
+  <si>
+    <t>/:idCarr</t>
+  </si>
+  <si>
+    <t>Devuelve el carrito pedido. Como parametro, hay que pasarle el mail del usuario. Si se le pasa un usuario que no existe, devuelve mensaje de error.</t>
+  </si>
+  <si>
+    <t>Crea un nuevo carrito, pasandole en el body el username. Debería funcionar así le pase un string o un numero.</t>
+  </si>
+  <si>
+    <t>Elimina un carrito. Probar si se le pasa un usuario correcto, uno que no existe, y un par de numeros.</t>
+  </si>
+  <si>
+    <t>/:idCarr/productos/:idProd</t>
+  </si>
+  <si>
+    <t>Agrega productos a un carrito. Comprobar si el carrito es correcto, no existe, o ingreso un string. Comprobar si el producto es correcto, no existe o es un string.</t>
+  </si>
+  <si>
+    <t>/:idCarr/productos</t>
+  </si>
+  <si>
+    <t>Trae los productos de un carrito. Probar si ingresamos usuario valido, que no existe e invalido. Ver que pasa si el carrito tiene cosas o esta vacio.</t>
+  </si>
+  <si>
+    <t>Elimina productos de un carrito. Comprobar si el carrito es correcto, no existe, o ingreso un string. Comprobar si el producto es correcto, no existe o es un string. Comprobar si el carrito esta vacio.</t>
+  </si>
+  <si>
+    <t>/:idCarr/confirmar</t>
+  </si>
+  <si>
+    <t>Confirma la compra y devuelve los productos adquiridos. Probar si ingreso un usuario valido, no valido e inexistente.</t>
+  </si>
+  <si>
+    <t>Ver como ingreso en Postman un req.user</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
+  </si>
+  <si>
+    <t>/compra/realizada/muchas/gracias</t>
+  </si>
+  <si>
+    <t>Devuelve un HTML con mensaje de compra realizada</t>
+  </si>
+  <si>
+    <t>/vaciar</t>
+  </si>
+  <si>
+    <t>Vacia el carrito del usuario, que se pasa por body. Verificar con usuario valido, no valido e inexistente. Debe devolver el usuario completo con carrito vacio</t>
   </si>
 </sst>
 </file>
@@ -109,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -145,6 +206,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF38AC4-C744-4BDE-A246-7C226FA981F1}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,4 +626,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80009AE-E81A-4ED1-88E8-0DA4E366058C}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="45.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>